<commit_message>
circuler graoh + image_url extraction
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\proyectos_varios\my_spotify_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA55A84-586C-464D-A6CC-ED87D5DDAE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBEE95C-2E88-4A03-83BA-C0E0D7FE8784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CE199CE-C18F-4379-A39D-B9D68E56191F}"/>
+    <workbookView xWindow="792" yWindow="0" windowWidth="17304" windowHeight="8892" xr2:uid="{2CE199CE-C18F-4379-A39D-B9D68E56191F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>image</t>
   </si>
   <si>
-    <t>https://o.scdn.co/image/ab67616d0000b27393e68ede7aca08e67e49c46d</t>
+    <t>//i.imgur.com/UxwnWnIb.jpg</t>
+  </si>
+  <si>
+    <t>//i.imgur.com/Or0O3Hob.jpg</t>
+  </si>
+  <si>
+    <t>//i.imgur.com/aJTAHiWb.jpg</t>
+  </si>
+  <si>
+    <t>//i.imgur.com/KpI0LyKb.jpg</t>
+  </si>
+  <si>
+    <t>//i.imgur.com/fpG0m7Jb.jpg</t>
+  </si>
+  <si>
+    <t>//i.imgur.com/D9heDsUb.jpg</t>
+  </si>
+  <si>
+    <t>//i.imgur.com/jZeZz0qb.jpg</t>
+  </si>
+  <si>
+    <t>//i.imgur.com/iiCBuzvb.jpg</t>
+  </si>
+  <si>
+    <t>//i.imgur.com/skS4fTJb.jpg</t>
   </si>
 </sst>
 </file>
@@ -404,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E1DB8B-89D6-4B77-BD8D-736C118C49A6}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,8 +446,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>